<commit_message>
Kommentare eingefügt. Nichts verändert
</commit_message>
<xml_diff>
--- a/Docs/Corvin/Datenkatalog_kommentare_v1.xlsx
+++ b/Docs/Corvin/Datenkatalog_kommentare_v1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\GitHub\InfoSys-Lab\Docs\Corvin\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entity" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,8 @@
     <sheet name="Attributes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sebastian</author>
   </authors>
   <commentList>
-    <comment ref="B9" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,12 +62,46 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Michi .</author>
+  </authors>
+  <commentList>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{965405B0-A77F-45D4-B9E7-3F88692F9B8E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michi .:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Doppelt?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sebastian</author>
   </authors>
   <commentList>
-    <comment ref="B7" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -89,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -110,11 +149,32 @@
           </rPr>
           <t xml:space="preserve">
 Attribut hinzufügen: "SWS" (int) nullable
-"Labor" (Boolean)not nullable</t>
+"Labor" (Boolean)not nullable
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+wer darf/muss die VL besuchen</t>
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -148,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -172,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0">
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -557,8 +617,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,6 +650,19 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -925,27 +998,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="59.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -956,7 +1029,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -967,7 +1040,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -978,7 +1051,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -986,7 +1059,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -994,7 +1067,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1002,7 +1075,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1010,7 +1083,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1018,7 +1091,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1026,7 +1099,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1034,22 +1107,22 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43037</v>
       </c>
@@ -1064,14 +1137,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" style="1"/>
@@ -1082,7 +1155,7 @@
     <col min="7" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1102,7 +1175,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60">
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1122,7 +1195,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -1139,7 +1212,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1159,7 +1232,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="90">
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -1179,7 +1252,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -1193,7 +1266,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1207,7 +1280,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -1224,7 +1297,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1241,7 +1314,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60">
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1261,7 +1334,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="60">
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1283,25 +1356,26 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="4" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1327,7 +1401,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1353,7 +1427,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>48</v>
       </c>
@@ -1376,7 +1450,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>49</v>
       </c>
@@ -1399,7 +1473,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>50</v>
       </c>
@@ -1422,7 +1496,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>51</v>
       </c>
@@ -1445,7 +1519,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>52</v>
       </c>
@@ -1468,7 +1542,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1494,7 +1568,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1520,7 +1594,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>54</v>
       </c>
@@ -1543,7 +1617,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1569,7 +1643,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>56</v>
       </c>
@@ -1592,7 +1666,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1618,7 +1692,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>58</v>
       </c>
@@ -1641,7 +1715,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>57</v>
       </c>
@@ -1664,7 +1738,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1690,7 +1764,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>60</v>
       </c>
@@ -1713,7 +1787,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>61</v>
       </c>
@@ -1736,7 +1810,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1762,12 +1836,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>43037</v>
       </c>
@@ -1775,12 +1849,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>105</v>
       </c>
@@ -1800,7 +1874,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>107</v>
       </c>
@@ -1820,7 +1894,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>110</v>
       </c>

</xml_diff>

<commit_message>
added mapping between user views and entities
</commit_message>
<xml_diff>
--- a/Docs/Corvin/Datenkatalog_kommentare_v1.xlsx
+++ b/Docs/Corvin/Datenkatalog_kommentare_v1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\InfoSys-Lab\Docs\Corvin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\hs-esslingen\Unterrichtsfächer\7. Semester\Infosys\GitRepo\InfoSys-Lab\Docs\Corvin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Entity" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sebastian</author>
   </authors>
   <commentList>
-    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
+    <comment ref="C17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -380,7 +380,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -784,7 +784,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -902,11 +902,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,10 +1105,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>

</xml_diff>